<commit_message>
final errors for piet
</commit_message>
<xml_diff>
--- a/cyclesNN.xlsx
+++ b/cyclesNN.xlsx
@@ -423,67 +423,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>11.53052756061517</v>
+        <v>0.7724775713279004</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10.93784774507678</v>
+        <v>0.732260308402072</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.824699703324557</v>
+        <v>0.2534333533236305</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.084127482150452</v>
+        <v>0.1276061961020767</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>13.67005166098647</v>
+        <v>0.8962634008536721</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>11.55235464607599</v>
+        <v>0.7739018424399541</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.952953536732465</v>
+        <v>0.1223483126088004</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5.021342762815148</v>
+        <v>0.2652424226402139</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>15.78071723416038</v>
+        <v>1.000150259811752</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>29.83589564571087</v>
+        <v>1.728893897005647</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>14.49096695034479</v>
+        <v>0.9377931549521943</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>28.15119597635282</v>
+        <v>1.633505894680542</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>30.65662274723461</v>
+        <v>1.7764735337147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>